<commit_message>
change the splitting train_val method
</commit_message>
<xml_diff>
--- a/Analysis/CrowdData/attr_funct.xlsx
+++ b/Analysis/CrowdData/attr_funct.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8775" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8775" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -17,18 +17,19 @@
     <sheet name="label sampling" sheetId="4" r:id="rId3"/>
     <sheet name="sampling fold 1" sheetId="5" r:id="rId4"/>
     <sheet name="confusion_matrix" sheetId="2" r:id="rId5"/>
+    <sheet name="select_loc_for_val" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="8" r:id="rId8"/>
+    <pivotCache cacheId="5" r:id="rId7"/>
+    <pivotCache cacheId="6" r:id="rId8"/>
+    <pivotCache cacheId="7" r:id="rId9"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>loc_id</t>
   </si>
@@ -91,6 +92,9 @@
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t>attractiveness</t>
   </si>
 </sst>
 </file>
@@ -5582,7 +5586,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -5665,7 +5669,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K1:L7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -5743,7 +5747,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G1:M6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisCol" dataField="1" subtotalTop="0" showAll="0">
@@ -5831,7 +5835,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O202" totalsRowShown="0">
-  <autoFilter ref="A1:O202"/>
+  <autoFilter ref="A1:O202">
+    <filterColumn colId="10">
+      <filters>
+        <filter val="5"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:O202">
     <sortCondition ref="A1:A202"/>
   </sortState>
@@ -6279,7 +6289,7 @@
   <dimension ref="A1:O205"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A1:O41"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6335,7 +6345,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -6386,7 +6396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -6437,7 +6447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -6488,7 +6498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -6539,7 +6549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -6590,7 +6600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>21</v>
       </c>
@@ -6641,7 +6651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>25</v>
       </c>
@@ -6743,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>28</v>
       </c>
@@ -6794,7 +6804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>30</v>
       </c>
@@ -6845,7 +6855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>34</v>
       </c>
@@ -6896,7 +6906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>35</v>
       </c>
@@ -6947,7 +6957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>40</v>
       </c>
@@ -6998,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>43</v>
       </c>
@@ -7049,7 +7059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>51</v>
       </c>
@@ -7100,7 +7110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>52</v>
       </c>
@@ -7151,7 +7161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>61</v>
       </c>
@@ -7202,7 +7212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>64</v>
       </c>
@@ -7253,7 +7263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>75</v>
       </c>
@@ -7304,7 +7314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>93</v>
       </c>
@@ -7355,7 +7365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>201</v>
       </c>
@@ -7406,7 +7416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>202</v>
       </c>
@@ -7457,7 +7467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>203</v>
       </c>
@@ -7508,7 +7518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>205</v>
       </c>
@@ -7559,7 +7569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>206</v>
       </c>
@@ -7610,7 +7620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>208</v>
       </c>
@@ -7661,7 +7671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>209</v>
       </c>
@@ -7712,7 +7722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>210</v>
       </c>
@@ -7763,7 +7773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>212</v>
       </c>
@@ -7814,7 +7824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>213</v>
       </c>
@@ -7865,7 +7875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>215</v>
       </c>
@@ -7916,7 +7926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>216</v>
       </c>
@@ -7967,7 +7977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>217</v>
       </c>
@@ -8018,7 +8028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>220</v>
       </c>
@@ -8069,7 +8079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>221</v>
       </c>
@@ -8120,7 +8130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>222</v>
       </c>
@@ -8171,7 +8181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>223</v>
       </c>
@@ -8222,7 +8232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>224</v>
       </c>
@@ -8273,7 +8283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>225</v>
       </c>
@@ -8324,7 +8334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>226</v>
       </c>
@@ -8375,7 +8385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>228</v>
       </c>
@@ -8426,7 +8436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>229</v>
       </c>
@@ -8477,7 +8487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>251</v>
       </c>
@@ -8528,7 +8538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>252</v>
       </c>
@@ -8579,7 +8589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>253</v>
       </c>
@@ -8630,7 +8640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>271</v>
       </c>
@@ -8681,7 +8691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>272</v>
       </c>
@@ -8732,7 +8742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>273</v>
       </c>
@@ -8783,7 +8793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>274</v>
       </c>
@@ -8834,7 +8844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>277</v>
       </c>
@@ -8885,7 +8895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>304</v>
       </c>
@@ -8936,7 +8946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>307</v>
       </c>
@@ -8987,7 +8997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>308</v>
       </c>
@@ -9038,7 +9048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>310</v>
       </c>
@@ -9089,7 +9099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>311</v>
       </c>
@@ -9140,7 +9150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>313</v>
       </c>
@@ -9191,7 +9201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>314</v>
       </c>
@@ -9242,7 +9252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>315</v>
       </c>
@@ -9293,7 +9303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>319</v>
       </c>
@@ -9344,7 +9354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>320</v>
       </c>
@@ -9395,7 +9405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>322</v>
       </c>
@@ -9446,7 +9456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>323</v>
       </c>
@@ -9497,7 +9507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>324</v>
       </c>
@@ -9548,7 +9558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>326</v>
       </c>
@@ -9599,7 +9609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>328</v>
       </c>
@@ -9650,7 +9660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>329</v>
       </c>
@@ -9701,7 +9711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>330</v>
       </c>
@@ -9752,7 +9762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>331</v>
       </c>
@@ -9803,7 +9813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>333</v>
       </c>
@@ -9854,7 +9864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>334</v>
       </c>
@@ -9905,7 +9915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>335</v>
       </c>
@@ -9956,7 +9966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>336</v>
       </c>
@@ -10007,7 +10017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>337</v>
       </c>
@@ -10058,7 +10068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>338</v>
       </c>
@@ -10109,7 +10119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>341</v>
       </c>
@@ -10160,7 +10170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>342</v>
       </c>
@@ -10211,7 +10221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>343</v>
       </c>
@@ -10262,7 +10272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>344</v>
       </c>
@@ -10313,7 +10323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>345</v>
       </c>
@@ -10364,7 +10374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>346</v>
       </c>
@@ -10415,7 +10425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>402</v>
       </c>
@@ -10466,7 +10476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>405</v>
       </c>
@@ -10517,7 +10527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>407</v>
       </c>
@@ -10568,7 +10578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>409</v>
       </c>
@@ -10619,7 +10629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>414</v>
       </c>
@@ -10670,7 +10680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>415</v>
       </c>
@@ -10721,7 +10731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>416</v>
       </c>
@@ -10772,7 +10782,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>418</v>
       </c>
@@ -10823,7 +10833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>421</v>
       </c>
@@ -10874,7 +10884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>422</v>
       </c>
@@ -10925,7 +10935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>425</v>
       </c>
@@ -10976,7 +10986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>426</v>
       </c>
@@ -11027,7 +11037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>427</v>
       </c>
@@ -11078,7 +11088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>428</v>
       </c>
@@ -11129,7 +11139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>429</v>
       </c>
@@ -11180,7 +11190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>430</v>
       </c>
@@ -11231,7 +11241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>432</v>
       </c>
@@ -11282,7 +11292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>434</v>
       </c>
@@ -11333,7 +11343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>436</v>
       </c>
@@ -11384,7 +11394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>437</v>
       </c>
@@ -11435,7 +11445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>438</v>
       </c>
@@ -11486,7 +11496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>439</v>
       </c>
@@ -11537,7 +11547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>443</v>
       </c>
@@ -11588,7 +11598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>444</v>
       </c>
@@ -11639,7 +11649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>448</v>
       </c>
@@ -11690,7 +11700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>449</v>
       </c>
@@ -11741,7 +11751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>453</v>
       </c>
@@ -11792,7 +11802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>454</v>
       </c>
@@ -11843,7 +11853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>459</v>
       </c>
@@ -11894,7 +11904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>465</v>
       </c>
@@ -11945,7 +11955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>466</v>
       </c>
@@ -11996,7 +12006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>467</v>
       </c>
@@ -12047,7 +12057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>472</v>
       </c>
@@ -12098,7 +12108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>473</v>
       </c>
@@ -12149,7 +12159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>476</v>
       </c>
@@ -12200,7 +12210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>477</v>
       </c>
@@ -12251,7 +12261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>479</v>
       </c>
@@ -12302,7 +12312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>481</v>
       </c>
@@ -12353,7 +12363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>484</v>
       </c>
@@ -12404,7 +12414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>485</v>
       </c>
@@ -12455,7 +12465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>492</v>
       </c>
@@ -12506,7 +12516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>496</v>
       </c>
@@ -12557,7 +12567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>497</v>
       </c>
@@ -12608,7 +12618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>499</v>
       </c>
@@ -12659,7 +12669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>500</v>
       </c>
@@ -12710,7 +12720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>503</v>
       </c>
@@ -12812,7 +12822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>508</v>
       </c>
@@ -12863,7 +12873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>511</v>
       </c>
@@ -12914,7 +12924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>512</v>
       </c>
@@ -12965,7 +12975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>514</v>
       </c>
@@ -13016,7 +13026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>515</v>
       </c>
@@ -13067,7 +13077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>516</v>
       </c>
@@ -13118,7 +13128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>517</v>
       </c>
@@ -13169,7 +13179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>520</v>
       </c>
@@ -13220,7 +13230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>523</v>
       </c>
@@ -13271,7 +13281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>527</v>
       </c>
@@ -13373,7 +13383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>530</v>
       </c>
@@ -13424,7 +13434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>533</v>
       </c>
@@ -13475,7 +13485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>536</v>
       </c>
@@ -13526,7 +13536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>538</v>
       </c>
@@ -13577,7 +13587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>539</v>
       </c>
@@ -13628,7 +13638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>540</v>
       </c>
@@ -13679,7 +13689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>547</v>
       </c>
@@ -13730,7 +13740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>548</v>
       </c>
@@ -13781,7 +13791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>555</v>
       </c>
@@ -13832,7 +13842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>556</v>
       </c>
@@ -13883,7 +13893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>559</v>
       </c>
@@ -13934,7 +13944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>561</v>
       </c>
@@ -13985,7 +13995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>564</v>
       </c>
@@ -14036,7 +14046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>567</v>
       </c>
@@ -14087,7 +14097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>569</v>
       </c>
@@ -14138,7 +14148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>570</v>
       </c>
@@ -14189,7 +14199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>578</v>
       </c>
@@ -14240,7 +14250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>579</v>
       </c>
@@ -14291,7 +14301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>582</v>
       </c>
@@ -14342,7 +14352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>587</v>
       </c>
@@ -14393,7 +14403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>589</v>
       </c>
@@ -14444,7 +14454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>594</v>
       </c>
@@ -14495,7 +14505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>595</v>
       </c>
@@ -14546,7 +14556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>598</v>
       </c>
@@ -14597,7 +14607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>599</v>
       </c>
@@ -14648,7 +14658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>600</v>
       </c>
@@ -14699,7 +14709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>602</v>
       </c>
@@ -14750,7 +14760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>606</v>
       </c>
@@ -14801,7 +14811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>607</v>
       </c>
@@ -14852,7 +14862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>610</v>
       </c>
@@ -14903,7 +14913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>611</v>
       </c>
@@ -14954,7 +14964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>612</v>
       </c>
@@ -15005,7 +15015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>615</v>
       </c>
@@ -15056,7 +15066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>620</v>
       </c>
@@ -15107,7 +15117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>623</v>
       </c>
@@ -15158,7 +15168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>624</v>
       </c>
@@ -15209,7 +15219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>628</v>
       </c>
@@ -15260,7 +15270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>634</v>
       </c>
@@ -15311,7 +15321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>640</v>
       </c>
@@ -15362,7 +15372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>641</v>
       </c>
@@ -15413,7 +15423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>642</v>
       </c>
@@ -15464,7 +15474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>644</v>
       </c>
@@ -15515,7 +15525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>646</v>
       </c>
@@ -15566,7 +15576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>649</v>
       </c>
@@ -15617,7 +15627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>650</v>
       </c>
@@ -15668,7 +15678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>653</v>
       </c>
@@ -15719,7 +15729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>654</v>
       </c>
@@ -15770,7 +15780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>655</v>
       </c>
@@ -15821,7 +15831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>662</v>
       </c>
@@ -15923,7 +15933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>668</v>
       </c>
@@ -15974,7 +15984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>669</v>
       </c>
@@ -16025,7 +16035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>670</v>
       </c>
@@ -16076,7 +16086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>673</v>
       </c>
@@ -16127,7 +16137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>675</v>
       </c>
@@ -16178,7 +16188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>681</v>
       </c>
@@ -16229,7 +16239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>684</v>
       </c>
@@ -16280,7 +16290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>685</v>
       </c>
@@ -16331,7 +16341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>686</v>
       </c>
@@ -16382,7 +16392,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>687</v>
       </c>
@@ -16433,7 +16443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>689</v>
       </c>
@@ -16484,7 +16494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>699</v>
       </c>
@@ -16535,7 +16545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>9999</v>
       </c>
@@ -16615,7 +16625,7 @@
   <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C14"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17801,8 +17811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20748,4 +20758,350 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection sqref="A1:A41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>220</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="16">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="16">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>51</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="16">
+        <v>52</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>203</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="16">
+        <v>206</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>212</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
+        <v>216</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>64</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>201</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>208</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>210</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="16">
+        <v>222</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>223</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="16">
+        <v>225</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>252</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="16">
+        <v>271</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>277</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="16">
+        <v>307</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="16">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
+        <v>25</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="17">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
+        <v>61</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <v>75</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="16">
+        <v>93</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <v>202</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="16">
+        <v>205</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
+        <v>209</v>
+      </c>
+      <c r="B38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="16">
+        <v>213</v>
+      </c>
+      <c r="B39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
+        <v>215</v>
+      </c>
+      <c r="B40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="22">
+        <v>26</v>
+      </c>
+      <c r="B41">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add prepare features with generator
</commit_message>
<xml_diff>
--- a/Analysis/CrowdData/attr_funct.xlsx
+++ b/Analysis/CrowdData/attr_funct.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8775" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="8775" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -18,23 +18,24 @@
     <sheet name="confusion_matrix" sheetId="2" r:id="rId4"/>
     <sheet name="confmat_detail" sheetId="7" r:id="rId5"/>
     <sheet name="confmat_lowvar" sheetId="9" r:id="rId6"/>
-    <sheet name="select_loc_for_val" sheetId="6" r:id="rId7"/>
+    <sheet name="select_loc_for_val_lowvar" sheetId="6" r:id="rId7"/>
+    <sheet name="loc_for_val" sheetId="10" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">confmat_detail!$AA$2:$AH$2</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="3" r:id="rId9"/>
-    <pivotCache cacheId="4" r:id="rId10"/>
-    <pivotCache cacheId="5" r:id="rId11"/>
+    <pivotCache cacheId="13" r:id="rId9"/>
+    <pivotCache cacheId="14" r:id="rId10"/>
+    <pivotCache cacheId="15" r:id="rId11"/>
+    <pivotCache cacheId="16" r:id="rId12"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="167">
   <si>
     <t>loc_id</t>
   </si>
@@ -94,9 +95,6 @@
   </si>
   <si>
     <t>Count of loc_id</t>
-  </si>
-  <si>
-    <t>count</t>
   </si>
   <si>
     <t>attractiveness</t>
@@ -523,6 +521,21 @@
   </si>
   <si>
     <t>variance</t>
+  </si>
+  <si>
+    <t># all locations</t>
+  </si>
+  <si>
+    <t>selected for validation (20%)</t>
+  </si>
+  <si>
+    <t># images in validation dataset</t>
+  </si>
+  <si>
+    <t>#golden images for validation</t>
+  </si>
+  <si>
+    <t># images from selected locations</t>
   </si>
 </sst>
 </file>
@@ -1223,21 +1236,7 @@
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1264,7 +1263,21 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -7539,7 +7552,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -7625,7 +7638,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="A3:H79" firstHeaderRow="1" firstDataRow="2" firstDataCol="3"/>
   <pivotFields count="18">
     <pivotField dataField="1" compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -8276,7 +8289,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G1:M6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisCol" dataField="1" subtotalTop="0" showAll="0">
@@ -8363,7 +8376,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0">
   <location ref="M1:T25" firstHeaderRow="0" firstDataRow="1" firstDataCol="3"/>
   <pivotFields count="9">
     <pivotField compact="0" outline="0" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -8639,7 +8652,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="H1:M18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -8788,29 +8801,29 @@
     <tableColumn id="9" name="lab3"/>
     <tableColumn id="10" name="lab4"/>
     <tableColumn id="11" name="lab_loc"/>
-    <tableColumn id="12" name="avg_lab" dataDxfId="10">
+    <tableColumn id="12" name="avg_lab" dataDxfId="8">
       <calculatedColumnFormula>AVERAGE(Table1[[#This Row],[lab1]:[lab4]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Column1" dataDxfId="9"/>
-    <tableColumn id="13" name="delta" dataDxfId="8">
+    <tableColumn id="16" name="Column1" dataDxfId="7"/>
+    <tableColumn id="13" name="delta" dataDxfId="6">
       <calculatedColumnFormula>ABS(Table1[[#This Row],[lab_loc]]-Table1[[#This Row],[avg_lab]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="lowconf" dataDxfId="7">
+    <tableColumn id="14" name="lowconf" dataDxfId="5">
       <calculatedColumnFormula>COUNTIF(Table1[[#This Row],[var1]:[var4]],"&gt;1")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="avg_lab_rounded" dataDxfId="6">
+    <tableColumn id="17" name="avg_lab_rounded" dataDxfId="4">
       <calculatedColumnFormula>ROUND(Table1[[#This Row],[avg_lab]],0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="labels" dataDxfId="5">
+    <tableColumn id="18" name="labels" dataDxfId="3">
       <calculatedColumnFormula>Table1[[#This Row],[lab1]]&amp;" "&amp;Table1[[#This Row],[lab2]]&amp;" "&amp;Table1[[#This Row],[lab3]]&amp;" "&amp;Table1[[#This Row],[lab4]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="correct?" dataDxfId="4">
+    <tableColumn id="20" name="correct?" dataDxfId="2">
       <calculatedColumnFormula>IF(Table1[[#This Row],[avg_lab_rounded]]=Table1[[#This Row],[lab_loc]],1,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="error^2" dataDxfId="3">
+    <tableColumn id="19" name="error^2" dataDxfId="1">
       <calculatedColumnFormula>(Table1[[#This Row],[lab_loc]]-Table1[[#This Row],[avg_lab]])^2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="lowcon_loc" dataDxfId="2"/>
+    <tableColumn id="15" name="lowcon_loc" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9256,13 +9269,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -9282,7 +9295,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5">
         <v>1.75</v>
@@ -9300,7 +9313,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6">
         <v>1.75</v>
@@ -9318,7 +9331,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7">
         <v>2.5</v>
@@ -9336,7 +9349,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8">
         <v>1.5</v>
@@ -9354,7 +9367,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9">
         <v>1.5</v>
@@ -9372,7 +9385,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10">
         <v>1.75</v>
@@ -9390,7 +9403,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -9408,7 +9421,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12">
         <v>1.75</v>
@@ -9426,7 +9439,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13">
         <v>1.75</v>
@@ -9446,7 +9459,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -9466,7 +9479,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15">
         <v>2.25</v>
@@ -9484,7 +9497,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16">
         <v>2.5</v>
@@ -9504,7 +9517,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17">
         <v>2</v>
@@ -9522,7 +9535,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>2.25</v>
@@ -9542,7 +9555,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19">
         <v>2.5</v>
@@ -9562,7 +9575,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20">
         <v>2.75</v>
@@ -9580,7 +9593,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21">
         <v>2.75</v>
@@ -9598,7 +9611,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -9616,7 +9629,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23">
         <v>2.25</v>
@@ -9636,7 +9649,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24">
         <v>2.5</v>
@@ -9654,7 +9667,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25">
         <v>2.5</v>
@@ -9672,7 +9685,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26">
         <v>2.75</v>
@@ -9692,7 +9705,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27">
         <v>3</v>
@@ -9710,7 +9723,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B28">
         <v>2.75</v>
@@ -9728,7 +9741,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B29">
         <v>2.75</v>
@@ -9746,7 +9759,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30">
         <v>2.5</v>
@@ -9764,7 +9777,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -9782,7 +9795,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32">
         <v>3.25</v>
@@ -9802,7 +9815,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B33">
         <v>3</v>
@@ -9820,7 +9833,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B34">
         <v>2.25</v>
@@ -9838,7 +9851,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35">
         <v>2</v>
@@ -9856,7 +9869,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36">
         <v>2.25</v>
@@ -9874,7 +9887,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37">
         <v>2.5</v>
@@ -9894,7 +9907,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>2.75</v>
@@ -9914,7 +9927,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -9932,7 +9945,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40">
         <v>2.75</v>
@@ -9950,7 +9963,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B41">
         <v>3</v>
@@ -9968,7 +9981,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B42">
         <v>3.25</v>
@@ -9986,7 +9999,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B43">
         <v>2.5</v>
@@ -10006,7 +10019,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44">
         <v>2.75</v>
@@ -10026,7 +10039,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45">
         <v>3</v>
@@ -10046,7 +10059,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B46">
         <v>2.75</v>
@@ -10064,7 +10077,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47">
         <v>3</v>
@@ -10086,7 +10099,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B48">
         <v>3.25</v>
@@ -10104,7 +10117,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B49">
         <v>3</v>
@@ -10122,7 +10135,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B50">
         <v>3.25</v>
@@ -10142,7 +10155,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B51">
         <v>3.5</v>
@@ -10160,7 +10173,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B52">
         <v>3</v>
@@ -10178,7 +10191,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B53">
         <v>3.25</v>
@@ -10196,7 +10209,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B54">
         <v>3</v>
@@ -10214,7 +10227,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B55">
         <v>3.25</v>
@@ -10234,7 +10247,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B56">
         <v>3.5</v>
@@ -10254,7 +10267,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B57">
         <v>3.25</v>
@@ -10272,7 +10285,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B58">
         <v>3.5</v>
@@ -10290,7 +10303,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B59">
         <v>3.75</v>
@@ -10310,7 +10323,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B60">
         <v>2.5</v>
@@ -10330,7 +10343,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B61">
         <v>2.75</v>
@@ -10348,7 +10361,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B62">
         <v>3</v>
@@ -10366,7 +10379,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B63">
         <v>3.25</v>
@@ -10384,7 +10397,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B64">
         <v>2.75</v>
@@ -10402,7 +10415,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B65">
         <v>3</v>
@@ -10420,7 +10433,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B66">
         <v>3.25</v>
@@ -10440,7 +10453,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B67">
         <v>3.5</v>
@@ -10458,7 +10471,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B68">
         <v>3.5</v>
@@ -10478,7 +10491,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B69">
         <v>3.75</v>
@@ -10498,7 +10511,7 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B70">
         <v>3.5</v>
@@ -10516,7 +10529,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B71">
         <v>3.25</v>
@@ -10534,7 +10547,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B72">
         <v>3.5</v>
@@ -10552,7 +10565,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B73">
         <v>3.75</v>
@@ -10570,7 +10583,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B74">
         <v>3.5</v>
@@ -10588,7 +10601,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B75">
         <v>3.75</v>
@@ -10606,7 +10619,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B76">
         <v>4</v>
@@ -10628,7 +10641,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B77">
         <v>4.25</v>
@@ -10646,7 +10659,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B78">
         <v>3.75</v>
@@ -10664,7 +10677,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B79">
         <v>4.25</v>
@@ -10689,8 +10702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10737,7 +10750,7 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
@@ -10746,16 +10759,16 @@
         <v>17</v>
       </c>
       <c r="P1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" t="s">
-        <v>54</v>
-      </c>
       <c r="R1" t="s">
+        <v>138</v>
+      </c>
+      <c r="S1" t="s">
         <v>139</v>
-      </c>
-      <c r="S1" t="s">
-        <v>140</v>
       </c>
       <c r="T1" t="s">
         <v>18</v>
@@ -24437,12 +24450,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N202">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:F202">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0.9</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24641,7 +24654,7 @@
       </c>
       <c r="C7" s="6"/>
       <c r="V7" s="31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="W7" s="31"/>
       <c r="X7" s="31"/>
@@ -24696,26 +24709,26 @@
         <v>4</v>
       </c>
       <c r="T9" s="31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="U9" s="2">
         <v>1</v>
       </c>
       <c r="V9" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W9" s="2" t="str">
         <f>ROUND(O9/201*100,1)&amp;"%"</f>
         <v>2%</v>
       </c>
       <c r="X9" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Y9" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Z9" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -24743,7 +24756,7 @@
         <v>2</v>
       </c>
       <c r="V10" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W10" s="2" t="str">
         <f>ROUND(O10/201*100,1)&amp;"%"</f>
@@ -24758,7 +24771,7 @@
         <v>0.5%</v>
       </c>
       <c r="Z10" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
@@ -24786,7 +24799,7 @@
         <v>3</v>
       </c>
       <c r="V11" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W11" s="2" t="str">
         <f>ROUND(O11/201*100,1)&amp;"%"</f>
@@ -24801,7 +24814,7 @@
         <v>2.5%</v>
       </c>
       <c r="Z11" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
@@ -24826,10 +24839,10 @@
         <v>4</v>
       </c>
       <c r="V12" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W12" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="X12" s="2" t="str">
         <f>ROUND(P12/201*100,1)&amp;"%"</f>
@@ -24840,7 +24853,7 @@
         <v>15.4%</v>
       </c>
       <c r="Z12" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -24862,20 +24875,20 @@
         <v>5</v>
       </c>
       <c r="V13" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W13" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="X13" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Y13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>2%</v>
       </c>
       <c r="Z13" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
@@ -26614,45 +26627,45 @@
       <c r="C1" s="24"/>
       <c r="D1" s="24"/>
       <c r="E1" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
       <c r="I1" s="25"/>
       <c r="M1" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N1" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="O1" s="14" t="s">
-        <v>27</v>
-      </c>
       <c r="P1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q1" t="s">
         <v>133</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>131</v>
+      </c>
+      <c r="S1" t="s">
         <v>134</v>
       </c>
-      <c r="R1" t="s">
-        <v>132</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>135</v>
       </c>
-      <c r="T1" t="s">
-        <v>136</v>
-      </c>
       <c r="V1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="W1">
         <f>133/201*100</f>
         <v>66.169154228855717</v>
       </c>
       <c r="AD1" s="26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AE1" s="27"/>
       <c r="AF1" s="27"/>
@@ -26661,16 +26674,16 @@
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="23" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" s="23" t="s">
-        <v>27</v>
       </c>
       <c r="E2" s="22">
         <v>1</v>
@@ -26688,7 +26701,7 @@
         <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N2">
         <v>1.5</v>
@@ -26704,20 +26717,20 @@
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
       <c r="V2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="W2">
         <f>SQRT(71/201)</f>
         <v>0.59433478010778673</v>
       </c>
       <c r="AA2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC2" t="s">
         <v>137</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>138</v>
       </c>
       <c r="AD2">
         <v>1</v>
@@ -26735,15 +26748,15 @@
         <v>5</v>
       </c>
       <c r="AI2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" s="22">
         <v>1.5</v>
@@ -26759,7 +26772,7 @@
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
       <c r="M3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N3">
         <v>1.75</v>
@@ -26775,14 +26788,14 @@
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
       <c r="V3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="W3">
         <f>SQRT(62.75/201)</f>
         <v>0.55873880724929792</v>
       </c>
       <c r="AA3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AB3">
         <v>1.5</v>
@@ -26800,10 +26813,10 @@
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="22">
         <v>1.5</v>
@@ -26819,7 +26832,7 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
       <c r="M4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N4">
         <v>1.75</v>
@@ -26837,7 +26850,7 @@
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
       <c r="AA4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AB4">
         <v>1.75</v>
@@ -26855,10 +26868,10 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5" s="22">
         <v>1.75</v>
@@ -26874,7 +26887,7 @@
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
       <c r="M5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -26890,7 +26903,7 @@
       <c r="S5" s="13"/>
       <c r="T5" s="13"/>
       <c r="AA5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AB5">
         <v>1.75</v>
@@ -26911,10 +26924,10 @@
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C6" s="22">
         <v>1.75</v>
@@ -26930,7 +26943,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
       <c r="M6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="N6">
         <v>2.25</v>
@@ -26946,7 +26959,7 @@
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
       <c r="AA6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AB6">
         <v>2</v>
@@ -26964,10 +26977,10 @@
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="22">
         <v>1.75</v>
@@ -26983,7 +26996,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
       <c r="M7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N7">
         <v>2.5</v>
@@ -26998,7 +27011,7 @@
       </c>
       <c r="T7" s="13"/>
       <c r="AA7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AB7">
         <v>2</v>
@@ -27019,10 +27032,10 @@
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="22">
         <v>1.75</v>
@@ -27038,7 +27051,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
       <c r="M8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N8">
         <v>3.5</v>
@@ -27054,7 +27067,7 @@
       </c>
       <c r="T8" s="13"/>
       <c r="AA8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB8">
         <v>2.25</v>
@@ -27072,10 +27085,10 @@
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="22">
         <v>1.75</v>
@@ -27093,7 +27106,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
       <c r="M9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N9">
         <v>2</v>
@@ -27111,7 +27124,7 @@
       <c r="S9" s="13"/>
       <c r="T9" s="13"/>
       <c r="AA9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AB9">
         <v>2.25</v>
@@ -27132,10 +27145,10 @@
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C10" s="22">
         <v>2</v>
@@ -27153,7 +27166,7 @@
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
       <c r="M10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N10">
         <v>2.25</v>
@@ -27171,7 +27184,7 @@
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
       <c r="AA10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AB10">
         <v>2.5</v>
@@ -27192,10 +27205,10 @@
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C11" s="22">
         <v>2</v>
@@ -27211,7 +27224,7 @@
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="M11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N11">
         <v>2.5</v>
@@ -27228,7 +27241,7 @@
       </c>
       <c r="T11" s="13"/>
       <c r="AA11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AB11">
         <v>2.5</v>
@@ -27252,10 +27265,10 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="22">
         <v>2</v>
@@ -27271,7 +27284,7 @@
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
       <c r="M12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N12">
         <v>2.5</v>
@@ -27286,7 +27299,7 @@
       <c r="S12" s="13"/>
       <c r="T12" s="13"/>
       <c r="AA12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AB12">
         <v>2.5</v>
@@ -27307,10 +27320,10 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C13" s="22">
         <v>2</v>
@@ -27326,7 +27339,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
       <c r="M13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="N13">
         <v>2.75</v>
@@ -27346,7 +27359,7 @@
       </c>
       <c r="T13" s="13"/>
       <c r="AA13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AB13">
         <v>2.75</v>
@@ -27370,10 +27383,10 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C14" s="22">
         <v>2.25</v>
@@ -27389,7 +27402,7 @@
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
       <c r="M14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N14">
         <v>3</v>
@@ -27405,7 +27418,7 @@
       </c>
       <c r="T14" s="13"/>
       <c r="AA14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AB14">
         <v>2.75</v>
@@ -27426,10 +27439,10 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C15" s="22">
         <v>2.25</v>
@@ -27447,7 +27460,7 @@
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
       <c r="M15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N15">
         <v>2.75</v>
@@ -27465,7 +27478,7 @@
       <c r="S15" s="13"/>
       <c r="T15" s="13"/>
       <c r="AA15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AB15">
         <v>3</v>
@@ -27483,10 +27496,10 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C16" s="22">
         <v>2.25</v>
@@ -27504,7 +27517,7 @@
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="M16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="N16">
         <v>3</v>
@@ -27524,7 +27537,7 @@
       </c>
       <c r="T16" s="13"/>
       <c r="AA16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AB16">
         <v>3</v>
@@ -27548,10 +27561,10 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C17" s="22">
         <v>2.25</v>
@@ -27567,7 +27580,7 @@
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
       <c r="M17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="N17">
         <v>3.25</v>
@@ -27587,7 +27600,7 @@
       </c>
       <c r="T17" s="13"/>
       <c r="AA17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB17">
         <v>3</v>
@@ -27611,10 +27624,10 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C18" s="22">
         <v>2.25</v>
@@ -27630,7 +27643,7 @@
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
       <c r="M18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N18">
         <v>3.5</v>
@@ -27646,7 +27659,7 @@
       </c>
       <c r="T18" s="13"/>
       <c r="AA18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB18">
         <v>3.25</v>
@@ -27670,10 +27683,10 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C19" s="22">
         <v>2.5</v>
@@ -27689,7 +27702,7 @@
       <c r="H19" s="22"/>
       <c r="I19" s="22"/>
       <c r="M19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N19">
         <v>3.75</v>
@@ -27705,7 +27718,7 @@
         <v>1</v>
       </c>
       <c r="AA19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AB19">
         <v>3.25</v>
@@ -27726,10 +27739,10 @@
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C20" s="22">
         <v>2.5</v>
@@ -27745,7 +27758,7 @@
       </c>
       <c r="I20" s="22"/>
       <c r="M20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N20">
         <v>3</v>
@@ -27765,7 +27778,7 @@
       </c>
       <c r="T20" s="13"/>
       <c r="AA20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB20">
         <v>3.5</v>
@@ -27783,10 +27796,10 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C21" s="22">
         <v>2.5</v>
@@ -27804,7 +27817,7 @@
       </c>
       <c r="I21" s="22"/>
       <c r="M21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N21">
         <v>3.5</v>
@@ -27822,7 +27835,7 @@
       </c>
       <c r="T21" s="13"/>
       <c r="AA21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB21">
         <v>3.5</v>
@@ -27840,10 +27853,10 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C22" s="22">
         <v>2.5</v>
@@ -27861,7 +27874,7 @@
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
       <c r="M22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="N22">
         <v>3.75</v>
@@ -27881,7 +27894,7 @@
         <v>1</v>
       </c>
       <c r="AA22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AB22">
         <v>3.5</v>
@@ -27902,10 +27915,10 @@
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" s="22">
         <v>2.5</v>
@@ -27923,7 +27936,7 @@
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="M23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="N23">
         <v>3.25</v>
@@ -27941,7 +27954,7 @@
       </c>
       <c r="T23" s="13"/>
       <c r="AA23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AB23">
         <v>3.75</v>
@@ -27959,10 +27972,10 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C24" s="22">
         <v>2.5</v>
@@ -27978,7 +27991,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
       <c r="M24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="N24">
         <v>4</v>
@@ -27998,7 +28011,7 @@
         <v>1</v>
       </c>
       <c r="AA24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AB24">
         <v>3.75</v>
@@ -28022,10 +28035,10 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B25" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" s="22">
         <v>2.5</v>
@@ -28041,7 +28054,7 @@
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
       <c r="M25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N25">
         <v>4.25</v>
@@ -28059,7 +28072,7 @@
         <v>1</v>
       </c>
       <c r="AA25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AB25">
         <v>4</v>
@@ -28083,10 +28096,10 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" s="22">
         <v>2.5</v>
@@ -28104,7 +28117,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
       <c r="AA26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AB26">
         <v>4.25</v>
@@ -28125,10 +28138,10 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C27" s="22">
         <v>2.5</v>
@@ -28148,10 +28161,10 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C28" s="22">
         <v>2.75</v>
@@ -28169,10 +28182,10 @@
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" s="22">
         <v>2.75</v>
@@ -28190,10 +28203,10 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30" s="22">
         <v>2.75</v>
@@ -28211,10 +28224,10 @@
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C31" s="22">
         <v>2.75</v>
@@ -28232,10 +28245,10 @@
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C32" s="22">
         <v>2.75</v>
@@ -28253,10 +28266,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C33" s="22">
         <v>2.75</v>
@@ -28274,10 +28287,10 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C34" s="22">
         <v>2.75</v>
@@ -28295,10 +28308,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C35" s="22">
         <v>2.75</v>
@@ -28318,10 +28331,10 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C36" s="22">
         <v>2.75</v>
@@ -28341,10 +28354,10 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C37" s="22">
         <v>2.75</v>
@@ -28364,10 +28377,10 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C38" s="22">
         <v>2.75</v>
@@ -28385,10 +28398,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C39" s="22">
         <v>3</v>
@@ -28406,10 +28419,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B40" s="22" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C40" s="22">
         <v>3</v>
@@ -28427,10 +28440,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C41" s="22">
         <v>3</v>
@@ -28448,10 +28461,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C42" s="22">
         <v>3</v>
@@ -28469,10 +28482,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C43" s="22">
         <v>3</v>
@@ -28490,10 +28503,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C44" s="22">
         <v>3</v>
@@ -28511,10 +28524,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C45" s="22">
         <v>3</v>
@@ -28534,10 +28547,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C46" s="22">
         <v>3</v>
@@ -28555,10 +28568,10 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C47" s="22">
         <v>3</v>
@@ -28576,10 +28589,10 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C48" s="22">
         <v>3</v>
@@ -28597,10 +28610,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C49" s="22">
         <v>3</v>
@@ -28618,10 +28631,10 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C50" s="22">
         <v>3</v>
@@ -28639,10 +28652,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C51" s="22">
         <v>3</v>
@@ -28664,10 +28677,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C52" s="22">
         <v>3.25</v>
@@ -28687,10 +28700,10 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C53" s="22">
         <v>3.25</v>
@@ -28708,10 +28721,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B54" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C54" s="22">
         <v>3.25</v>
@@ -28729,10 +28742,10 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C55" s="22">
         <v>3.25</v>
@@ -28750,10 +28763,10 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B56" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C56" s="22">
         <v>3.25</v>
@@ -28771,10 +28784,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C57" s="22">
         <v>3.25</v>
@@ -28792,10 +28805,10 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C58" s="22">
         <v>3.25</v>
@@ -28813,10 +28826,10 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C59" s="22">
         <v>3.25</v>
@@ -28836,10 +28849,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C60" s="22">
         <v>3.25</v>
@@ -28859,10 +28872,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C61" s="22">
         <v>3.25</v>
@@ -28882,10 +28895,10 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C62" s="22">
         <v>3.5</v>
@@ -28903,10 +28916,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C63" s="22">
         <v>3.5</v>
@@ -28926,10 +28939,10 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C64" s="22">
         <v>3.5</v>
@@ -28947,10 +28960,10 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C65" s="22">
         <v>3.5</v>
@@ -28968,10 +28981,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C66" s="22">
         <v>3.5</v>
@@ -28991,10 +29004,10 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C67" s="22">
         <v>3.5</v>
@@ -29012,10 +29025,10 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B68" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C68" s="22">
         <v>3.5</v>
@@ -29033,10 +29046,10 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C69" s="22">
         <v>3.5</v>
@@ -29054,10 +29067,10 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C70" s="22">
         <v>3.75</v>
@@ -29077,10 +29090,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C71" s="22">
         <v>3.75</v>
@@ -29100,10 +29113,10 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C72" s="22">
         <v>3.75</v>
@@ -29121,10 +29134,10 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C73" s="22">
         <v>3.75</v>
@@ -29142,10 +29155,10 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C74" s="22">
         <v>3.75</v>
@@ -29163,10 +29176,10 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C75" s="22">
         <v>4</v>
@@ -29188,10 +29201,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C76" s="22">
         <v>4.25</v>
@@ -29209,10 +29222,10 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C77" s="22">
         <v>4.25</v>
@@ -29262,10 +29275,10 @@
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>11</v>
@@ -29274,7 +29287,7 @@
         <v>10</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>15</v>
@@ -29282,10 +29295,10 @@
     </row>
     <row r="2" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="19">
         <v>1.75</v>
@@ -29314,10 +29327,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="19">
         <v>1.75</v>
@@ -29326,7 +29339,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I3" s="13">
         <v>2</v>
@@ -29340,10 +29353,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" s="19">
         <v>2</v>
@@ -29352,7 +29365,7 @@
         <v>2</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13">
@@ -29366,10 +29379,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="20">
         <v>2.25</v>
@@ -29378,7 +29391,7 @@
         <v>2</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13">
@@ -29392,10 +29405,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C6" s="20">
         <v>2.5</v>
@@ -29404,7 +29417,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I6" s="13"/>
       <c r="J6" s="13">
@@ -29418,10 +29431,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="20">
         <v>2.25</v>
@@ -29430,7 +29443,7 @@
         <v>2</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
@@ -29444,10 +29457,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C8" s="20">
         <v>2.25</v>
@@ -29456,7 +29469,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I8" s="13"/>
       <c r="J8" s="13">
@@ -29472,10 +29485,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="20">
         <v>2.5</v>
@@ -29484,7 +29497,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I9" s="13"/>
       <c r="J9" s="13">
@@ -29498,10 +29511,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C10" s="19">
         <v>2.5</v>
@@ -29510,7 +29523,7 @@
         <v>2</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
@@ -29524,10 +29537,10 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="19">
         <v>2.5</v>
@@ -29536,7 +29549,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="13">
@@ -29552,10 +29565,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C12" s="20">
         <v>2.5</v>
@@ -29564,7 +29577,7 @@
         <v>3</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I12" s="13"/>
       <c r="J12" s="13">
@@ -29582,10 +29595,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" s="19">
         <v>2.75</v>
@@ -29594,7 +29607,7 @@
         <v>2</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
@@ -29608,10 +29621,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C14" s="20">
         <v>2.75</v>
@@ -29620,7 +29633,7 @@
         <v>3</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
@@ -29634,10 +29647,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C15" s="19">
         <v>3</v>
@@ -29646,7 +29659,7 @@
         <v>4</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
@@ -29660,10 +29673,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C16" s="19">
         <v>3</v>
@@ -29672,7 +29685,7 @@
         <v>3</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I16" s="13"/>
       <c r="J16" s="13">
@@ -29688,10 +29701,10 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C17" s="20">
         <v>3.25</v>
@@ -29700,7 +29713,7 @@
         <v>4</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
@@ -29714,10 +29727,10 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18" s="20">
         <v>3</v>
@@ -29746,10 +29759,10 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C19" s="20">
         <v>2</v>
@@ -29760,10 +29773,10 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C20" s="19">
         <v>2.25</v>
@@ -29774,10 +29787,10 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C21" s="19">
         <v>2.5</v>
@@ -29788,10 +29801,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C22" s="19">
         <v>2.5</v>
@@ -29802,10 +29815,10 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C23" s="19">
         <v>2.75</v>
@@ -29816,10 +29829,10 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C24" s="20">
         <v>2.75</v>
@@ -29830,10 +29843,10 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C25" s="20">
         <v>3</v>
@@ -29844,10 +29857,10 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C26" s="20">
         <v>3</v>
@@ -29858,10 +29871,10 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C27" s="20">
         <v>2.5</v>
@@ -29872,10 +29885,10 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C28" s="19">
         <v>2.75</v>
@@ -29886,10 +29899,10 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C29" s="20">
         <v>2.75</v>
@@ -29900,10 +29913,10 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C30" s="19">
         <v>2.75</v>
@@ -29914,10 +29927,10 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C31" s="19">
         <v>3</v>
@@ -29928,10 +29941,10 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C32" s="19">
         <v>3</v>
@@ -29942,10 +29955,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C33" s="19">
         <v>3.25</v>
@@ -29956,10 +29969,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C34" s="20">
         <v>3.5</v>
@@ -29970,10 +29983,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C35" s="19">
         <v>2.75</v>
@@ -29984,10 +29997,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C36" s="20">
         <v>3.75</v>
@@ -29998,10 +30011,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C37" s="19">
         <v>3.75</v>
@@ -30012,10 +30025,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C38" s="19">
         <v>3.75</v>
@@ -30026,10 +30039,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C39" s="20">
         <v>4</v>
@@ -30040,10 +30053,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C40" s="20">
         <v>4</v>
@@ -30054,10 +30067,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C41" s="29">
         <v>4</v>
@@ -30068,7 +30081,7 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B45">
         <f>113/161</f>
@@ -30077,7 +30090,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B46">
         <f>43.8125/161</f>
@@ -30514,10 +30527,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30525,17 +30538,18 @@
     <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J1">
         <v>1</v>
@@ -30553,7 +30567,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>220</v>
       </c>
@@ -30566,7 +30580,7 @@
         <v>0.64</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>162</v>
       </c>
       <c r="J2">
         <v>4</v>
@@ -30583,8 +30597,12 @@
       <c r="N2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <f>SUM(J2:N2)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -30596,8 +30614,8 @@
         <f>VLOOKUP(A3,Table1[#All],6,FALSE)</f>
         <v>0.64</v>
       </c>
-      <c r="I3" s="16">
-        <v>0.2</v>
+      <c r="I3" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="J3" s="17">
         <f>20%*J2</f>
@@ -30618,8 +30636,12 @@
         <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <f>SUM(J3:N3)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>34</v>
       </c>
@@ -30631,8 +30653,12 @@
         <f>VLOOKUP(A4,Table1[#All],6,FALSE)</f>
         <v>0.159999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <f t="shared" ref="O4:O7" si="1">SUM(J4:N4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>40</v>
       </c>
@@ -30644,8 +30670,30 @@
         <f>VLOOKUP(A5,Table1[#All],6,FALSE)</f>
         <v>0.64</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J5" s="13">
+        <v>3</v>
+      </c>
+      <c r="K5" s="13">
+        <v>55</v>
+      </c>
+      <c r="L5" s="13">
+        <v>73</v>
+      </c>
+      <c r="M5" s="13">
+        <v>33</v>
+      </c>
+      <c r="N5" s="13">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>43</v>
       </c>
@@ -30657,8 +30705,30 @@
         <f>VLOOKUP(A6,Table1[#All],6,FALSE)</f>
         <v>0.64</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>165</v>
+      </c>
+      <c r="J6" s="13">
+        <v>0</v>
+      </c>
+      <c r="K6" s="13">
+        <v>0</v>
+      </c>
+      <c r="L6" s="13">
+        <v>2</v>
+      </c>
+      <c r="M6" s="13">
+        <v>3</v>
+      </c>
+      <c r="N6" s="13">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>51</v>
       </c>
@@ -30670,8 +30740,35 @@
         <f>VLOOKUP(A7,Table1[#All],6,FALSE)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>164</v>
+      </c>
+      <c r="J7">
+        <f>J5+J6</f>
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:N7" si="2">K5+K6</f>
+        <v>55</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>75</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>203</v>
       </c>
@@ -30684,7 +30781,7 @@
         <v>0.159999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>216</v>
       </c>
@@ -30697,7 +30794,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>217</v>
       </c>
@@ -30710,7 +30807,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>221</v>
       </c>
@@ -30723,7 +30820,7 @@
         <v>0.159999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>224</v>
       </c>
@@ -30736,7 +30833,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>272</v>
       </c>
@@ -30749,7 +30846,7 @@
         <v>0.159999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>322</v>
       </c>
@@ -30762,7 +30859,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>324</v>
       </c>
@@ -30775,7 +30872,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>6</v>
       </c>
@@ -31111,6 +31208,103 @@
       <c r="C41">
         <f>VLOOKUP(A41,Table1[#All],6,FALSE)</f>
         <v>0.24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O3" sqref="I1:O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J1">
+        <v>1</v>
+      </c>
+      <c r="K1">
+        <v>2</v>
+      </c>
+      <c r="L1">
+        <v>3</v>
+      </c>
+      <c r="M1">
+        <v>4</v>
+      </c>
+      <c r="N1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>70</v>
+      </c>
+      <c r="L2">
+        <v>64</v>
+      </c>
+      <c r="M2">
+        <v>58</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <f>SUM(J2:N2)</f>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I3" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="J3" s="17">
+        <f>20%*J2</f>
+        <v>0.8</v>
+      </c>
+      <c r="K3" s="17">
+        <v>13</v>
+      </c>
+      <c r="L3" s="17">
+        <f t="shared" ref="L3:N3" si="0">20%*L2</f>
+        <v>12.8</v>
+      </c>
+      <c r="M3" s="17">
+        <f t="shared" si="0"/>
+        <v>11.600000000000001</v>
+      </c>
+      <c r="N3" s="17">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="O3">
+        <f>SUM(J3:N3)</f>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>